<commit_message>
Removed specialized resource type for related items
</commit_message>
<xml_diff>
--- a/nr_vocabularies/fixtures/resource-types.xlsx
+++ b/nr_vocabularies/fixtures/resource-types.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="220">
   <si>
     <t>code</t>
   </si>
@@ -626,6 +626,147 @@
   </si>
   <si>
     <t>Ostatní</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_5ce6</t>
+  </si>
+  <si>
+    <t>source-code</t>
+  </si>
+  <si>
+    <t>Zdrojový kód</t>
+  </si>
+  <si>
+    <t>Source code</t>
+  </si>
+  <si>
+    <t>source code</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/QH80-2R4E</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>Časopis</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_0640</t>
+  </si>
+  <si>
+    <t>data-paper</t>
+  </si>
+  <si>
+    <t>Data paper</t>
+  </si>
+  <si>
+    <t>článek o datové sadě</t>
+  </si>
+  <si>
+    <t>data paper</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_beb9</t>
+  </si>
+  <si>
+    <t>DataPaper</t>
+  </si>
+  <si>
+    <t>data-management-plan</t>
+  </si>
+  <si>
+    <t>Data management plan</t>
+  </si>
+  <si>
+    <t>data management plan</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_ab20</t>
+  </si>
+  <si>
+    <t>OutputManagementPlan</t>
+  </si>
+  <si>
+    <t>interactive-resource</t>
+  </si>
+  <si>
+    <t>Interaktivní zdroj</t>
+  </si>
+  <si>
+    <t>Interactive resource</t>
+  </si>
+  <si>
+    <t>interactive resource</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_e9a0</t>
+  </si>
+  <si>
+    <t>InteractiveResource</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_1843</t>
+  </si>
+  <si>
+    <t>physical-object</t>
+  </si>
+  <si>
+    <t>Fyzický objekt</t>
+  </si>
+  <si>
+    <t>Physical object</t>
+  </si>
+  <si>
+    <t>PhysicalObject</t>
+  </si>
+  <si>
+    <t>patent</t>
+  </si>
+  <si>
+    <t>Patent</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_15cd</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>Norma</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>cartographic-material</t>
+  </si>
+  <si>
+    <t>Kartografický dokument</t>
+  </si>
+  <si>
+    <t>Cartographic material</t>
+  </si>
+  <si>
+    <t>mapy</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/resource_type/c_12cc</t>
   </si>
 </sst>
 </file>
@@ -687,7 +828,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -755,13 +896,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -816,8 +1044,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1901,7 +2156,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2943,147 +3198,393 @@
     </row>
     <row r="43" ht="15.6" customHeight="1">
       <c r="A43" s="10"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="5"/>
+      <c r="B43" t="s" s="15">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s" s="15">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s" s="15">
+        <v>38</v>
+      </c>
+      <c r="E43" t="s" s="15">
+        <v>39</v>
+      </c>
       <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
+      <c r="G43" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="H43" t="s" s="14">
+        <v>41</v>
+      </c>
+      <c r="I43" t="s" s="3">
+        <v>38</v>
+      </c>
       <c r="J43" s="5"/>
     </row>
     <row r="44" ht="15.6" customHeight="1">
       <c r="A44" s="10"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" t="s" s="3">
+        <v>173</v>
+      </c>
+      <c r="C44" t="s" s="15">
+        <v>174</v>
+      </c>
+      <c r="D44" t="s" s="15">
+        <v>174</v>
+      </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
+      <c r="G44" t="s" s="3">
+        <v>173</v>
+      </c>
+      <c r="H44" t="s" s="3">
+        <v>175</v>
+      </c>
+      <c r="I44" t="s" s="3">
+        <v>174</v>
+      </c>
       <c r="J44" s="5"/>
     </row>
     <row r="45" ht="15.6" customHeight="1">
       <c r="A45" s="10"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" t="s" s="15">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s" s="15">
+        <v>177</v>
+      </c>
+      <c r="D45" t="s" s="15">
+        <v>178</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
+      <c r="G45" t="s" s="3">
+        <v>179</v>
+      </c>
+      <c r="H45" t="s" s="3">
+        <v>180</v>
+      </c>
+      <c r="I45" t="s" s="3">
+        <v>103</v>
+      </c>
       <c r="J45" s="5"/>
     </row>
     <row r="46" ht="15.6" customHeight="1">
       <c r="A46" s="10"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="B46" t="s" s="15">
+        <v>181</v>
+      </c>
+      <c r="C46" t="s" s="15">
+        <v>182</v>
+      </c>
+      <c r="D46" t="s" s="15">
+        <v>183</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
+      <c r="G46" t="s" s="3">
+        <v>181</v>
+      </c>
+      <c r="H46" t="s" s="3">
+        <v>184</v>
+      </c>
+      <c r="I46" t="s" s="3">
+        <v>183</v>
+      </c>
       <c r="J46" s="5"/>
     </row>
     <row r="47" ht="15.6" customHeight="1">
       <c r="A47" s="10"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
+      <c r="B47" t="s" s="15">
+        <v>185</v>
+      </c>
+      <c r="C47" t="s" s="15">
+        <v>186</v>
+      </c>
+      <c r="D47" t="s" s="15">
+        <v>186</v>
+      </c>
+      <c r="E47" t="s" s="15">
+        <v>187</v>
+      </c>
       <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+      <c r="G47" t="s" s="3">
+        <v>188</v>
+      </c>
+      <c r="H47" t="s" s="3">
+        <v>189</v>
+      </c>
+      <c r="I47" t="s" s="3">
+        <v>190</v>
+      </c>
       <c r="J47" s="5"/>
     </row>
     <row r="48" ht="15.6" customHeight="1">
       <c r="A48" s="10"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="B48" t="s" s="15">
+        <v>191</v>
+      </c>
+      <c r="C48" t="s" s="15">
+        <v>192</v>
+      </c>
+      <c r="D48" t="s" s="15">
+        <v>192</v>
+      </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="9"/>
+      <c r="G48" t="s" s="3">
+        <v>193</v>
+      </c>
+      <c r="H48" t="s" s="3">
+        <v>194</v>
+      </c>
+      <c r="I48" t="s" s="18">
+        <v>195</v>
+      </c>
       <c r="J48" s="5"/>
     </row>
     <row r="49" ht="15.6" customHeight="1">
       <c r="A49" s="10"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+      <c r="B49" t="s" s="15">
+        <v>196</v>
+      </c>
+      <c r="C49" t="s" s="15">
+        <v>197</v>
+      </c>
+      <c r="D49" t="s" s="15">
+        <v>198</v>
+      </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
+      <c r="G49" t="s" s="15">
+        <v>199</v>
+      </c>
+      <c r="H49" t="s" s="3">
+        <v>200</v>
+      </c>
+      <c r="I49" t="s" s="3">
+        <v>201</v>
+      </c>
       <c r="J49" s="5"/>
     </row>
     <row r="50" ht="15.6" customHeight="1">
       <c r="A50" s="10"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="18"/>
+      <c r="B50" t="s" s="15">
+        <v>202</v>
+      </c>
+      <c r="C50" t="s" s="3">
+        <v>203</v>
+      </c>
+      <c r="D50" t="s" s="15">
+        <v>203</v>
+      </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
+      <c r="G50" t="s" s="3">
+        <v>156</v>
+      </c>
+      <c r="H50" t="s" s="3">
+        <v>204</v>
+      </c>
+      <c r="I50" t="s" s="3">
+        <v>203</v>
+      </c>
       <c r="J50" s="5"/>
     </row>
     <row r="51" ht="15.6" customHeight="1">
       <c r="A51" s="10"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="18"/>
+      <c r="B51" t="s" s="15">
+        <v>205</v>
+      </c>
+      <c r="C51" t="s" s="3">
+        <v>206</v>
+      </c>
+      <c r="D51" t="s" s="15">
+        <v>207</v>
+      </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
+      <c r="G51" t="s" s="3">
+        <v>156</v>
+      </c>
+      <c r="H51" t="s" s="3">
+        <v>204</v>
+      </c>
+      <c r="I51" t="s" s="3">
+        <v>208</v>
+      </c>
       <c r="J51" s="5"/>
     </row>
     <row r="52" ht="15.6" customHeight="1">
       <c r="A52" s="10"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="18"/>
+      <c r="B52" t="s" s="15">
+        <v>209</v>
+      </c>
+      <c r="C52" t="s" s="3">
+        <v>210</v>
+      </c>
+      <c r="D52" t="s" s="15">
+        <v>210</v>
+      </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
+      <c r="G52" t="s" s="3">
+        <v>209</v>
+      </c>
+      <c r="H52" t="s" s="3">
+        <v>211</v>
+      </c>
+      <c r="I52" t="s" s="3">
+        <v>35</v>
+      </c>
       <c r="J52" s="5"/>
     </row>
     <row r="53" ht="15.6" customHeight="1">
       <c r="A53" s="10"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="18"/>
+      <c r="B53" t="s" s="15">
+        <v>212</v>
+      </c>
+      <c r="C53" t="s" s="3">
+        <v>213</v>
+      </c>
+      <c r="D53" t="s" s="15">
+        <v>214</v>
+      </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
+      <c r="G53" t="s" s="3">
+        <v>156</v>
+      </c>
+      <c r="H53" t="s" s="3">
+        <v>204</v>
+      </c>
+      <c r="I53" t="s" s="3">
+        <v>214</v>
+      </c>
       <c r="J53" s="5"/>
     </row>
     <row r="54" ht="15.6" customHeight="1">
       <c r="A54" s="10"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="5"/>
+      <c r="B54" t="s" s="3">
+        <v>215</v>
+      </c>
+      <c r="C54" t="s" s="3">
+        <v>216</v>
+      </c>
+      <c r="D54" t="s" s="15">
+        <v>217</v>
+      </c>
+      <c r="E54" t="s" s="3">
+        <v>218</v>
+      </c>
       <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
+      <c r="G54" t="s" s="3">
+        <v>164</v>
+      </c>
+      <c r="H54" t="s" s="3">
+        <v>219</v>
+      </c>
+      <c r="I54" t="s" s="3">
+        <v>62</v>
+      </c>
       <c r="J54" s="5"/>
+    </row>
+    <row r="55" ht="15.6" customHeight="1">
+      <c r="A55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="21"/>
+    </row>
+    <row r="56" ht="15.6" customHeight="1">
+      <c r="A56" s="22"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="24"/>
+    </row>
+    <row r="57" ht="15.6" customHeight="1">
+      <c r="A57" s="22"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="24"/>
+    </row>
+    <row r="58" ht="15.6" customHeight="1">
+      <c r="A58" s="22"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="24"/>
+    </row>
+    <row r="59" ht="15.6" customHeight="1">
+      <c r="A59" s="22"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="24"/>
+    </row>
+    <row r="60" ht="15.6" customHeight="1">
+      <c r="A60" s="22"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="24"/>
+    </row>
+    <row r="61" ht="15.6" customHeight="1">
+      <c r="A61" s="22"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="24"/>
+    </row>
+    <row r="62" ht="15.6" customHeight="1">
+      <c r="A62" s="25"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3107,6 +3608,7 @@
     <hyperlink ref="H40" r:id="rId18" location="" tooltip="" display="http://purl.org/coar/resource_type/c_1843"/>
     <hyperlink ref="H41" r:id="rId19" location="" tooltip="" display="http://purl.org/coar/resource_type/c_1843"/>
     <hyperlink ref="H42" r:id="rId20" location="" tooltip="" display="http://purl.org/coar/resource_type/c_1843"/>
+    <hyperlink ref="H43" r:id="rId21" location="" tooltip="" display="http://purl.org/coar/resource_type/c_ddb1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>